<commit_message>
update for template examples resolving all within-template collisions
</commit_message>
<xml_diff>
--- a/template_examples/h_and_e_template.xlsx
+++ b/template_examples/h_and_e_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C763DD-78FE-BA4A-9FB2-FEC538053BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983C3E85-3C90-6942-A617-482CEB9AA2A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1360" windowWidth="14400" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8100" yWindow="24460" windowWidth="21380" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -1158,7 +1158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="289">
   <si>
     <t>#t</t>
   </si>
@@ -2003,9 +2003,6 @@
     <t>ship to</t>
   </si>
   <si>
-    <t>TTTPP801</t>
-  </si>
-  <si>
     <t>TRIALGROUP 1</t>
   </si>
   <si>
@@ -2015,9 +2012,6 @@
     <t>CTTTP08T1.00</t>
   </si>
   <si>
-    <t>TTTPP802</t>
-  </si>
-  <si>
     <t>TRIALGROUP 2</t>
   </si>
   <si>
@@ -2028,6 +2022,9 @@
   </si>
   <si>
     <t>A2</t>
+  </si>
+  <si>
+    <t>TTTPP8</t>
   </si>
 </sst>
 </file>
@@ -2180,9 +2177,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2191,6 +2185,9 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2546,10 +2543,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2558,7 +2555,7 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>275</v>
       </c>
     </row>
@@ -2569,7 +2566,7 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>276</v>
       </c>
     </row>
@@ -2580,7 +2577,7 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>3</v>
       </c>
     </row>
@@ -2591,7 +2588,7 @@
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2602,7 +2599,7 @@
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2613,7 +2610,7 @@
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2624,7 +2621,7 @@
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>277</v>
       </c>
     </row>
@@ -2635,7 +2632,7 @@
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>278</v>
       </c>
     </row>
@@ -2646,7 +2643,7 @@
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2657,7 +2654,7 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>37174</v>
       </c>
     </row>
@@ -2668,7 +2665,7 @@
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>37539</v>
       </c>
     </row>
@@ -2679,7 +2676,7 @@
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2690,7 +2687,7 @@
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>279</v>
       </c>
     </row>
@@ -2701,7 +2698,7 @@
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3723,8 +3720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3734,42 +3731,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -3877,25 +3874,25 @@
         <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="E3" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" t="s">
         <v>281</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>282</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>283</v>
-      </c>
-      <c r="H3" t="s">
-        <v>284</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K3" t="s">
         <v>213</v>
@@ -3972,22 +3969,22 @@
         <v>189</v>
       </c>
       <c r="E4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F4" t="s">
+        <v>284</v>
+      </c>
+      <c r="G4" t="s">
+        <v>282</v>
+      </c>
+      <c r="H4" t="s">
         <v>285</v>
-      </c>
-      <c r="F4" t="s">
-        <v>286</v>
-      </c>
-      <c r="G4" t="s">
-        <v>283</v>
-      </c>
-      <c r="H4" t="s">
-        <v>287</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K4" t="s">
         <v>213</v>

</xml_diff>